<commit_message>
join_form.jsp & MemberDAO upload
</commit_message>
<xml_diff>
--- a/01.Document/DB_TABLE_V2.0.0.xlsx
+++ b/01.Document/DB_TABLE_V2.0.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KH_SEMI\KickKick\01.Document\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KH_SEMI_WORKSPACE\KickKick\01.Document\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E65F4E51-AAAC-455A-A5B2-2C07A447CD94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD2B7D71-9D62-4DC6-A2F5-EA7F01EB0AF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5FBE2D67-92EF-4127-A433-F955F497CDE7}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="138">
   <si>
     <t>아이디</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -362,11 +362,6 @@
   </si>
   <si>
     <t>실력</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>1
-~</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -550,6 +545,20 @@
   </si>
   <si>
     <t>용병 등록 코드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>게시글 코드</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>FK
+NOT NULL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1
+~</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -850,26 +859,26 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1187,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C484617-72AE-4822-A547-3AE8808B7168}">
   <dimension ref="A1:X49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1243,38 +1252,38 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="G3" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="K3" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="L3" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="N3" s="9" t="s">
         <v>11</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="P3" s="6"/>
       <c r="R3" s="9" t="s">
         <v>12</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="T3" s="6"/>
     </row>
@@ -1295,16 +1304,16 @@
         <v>81</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>81</v>
       </c>
       <c r="I4" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="J4" s="7" t="s">
         <v>93</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>94</v>
       </c>
       <c r="K4" s="7" t="s">
         <v>81</v>
@@ -1358,42 +1367,42 @@
         <v>3</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="I6" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="L6" s="6"/>
       <c r="N6" s="9" t="s">
         <v>4</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P6" s="6"/>
       <c r="R6" s="9" t="s">
         <v>17</v>
       </c>
       <c r="S6" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="T6" s="10" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="2:24" ht="33" x14ac:dyDescent="0.3">
@@ -1404,10 +1413,10 @@
         <v>78</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F7" s="14" t="s">
         <v>78</v>
@@ -1606,7 +1615,7 @@
       <c r="K14" s="30"/>
       <c r="L14" s="31"/>
       <c r="N14" s="29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="O14" s="30"/>
       <c r="P14" s="31"/>
@@ -1636,7 +1645,7 @@
         <v>3</v>
       </c>
       <c r="P15" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="V15" s="12"/>
       <c r="W15" s="1"/>
@@ -1701,19 +1710,19 @@
         <v>18</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D19" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>20</v>
@@ -1726,10 +1735,10 @@
       </c>
       <c r="L19" s="6"/>
       <c r="N19" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="O19" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="P19" s="10" t="s">
         <v>19</v>
@@ -1790,29 +1799,29 @@
       <c r="T20" s="8"/>
     </row>
     <row r="21" spans="2:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="33" t="s">
+      <c r="B21" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="34"/>
-      <c r="E21" s="34"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="34"/>
-      <c r="H21" s="34"/>
-      <c r="I21" s="34"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34"/>
-      <c r="L21" s="35"/>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="33"/>
+      <c r="J21" s="33"/>
+      <c r="K21" s="33"/>
+      <c r="L21" s="34"/>
     </row>
     <row r="22" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B22" s="9" t="s">
         <v>23</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>20</v>
@@ -1849,35 +1858,35 @@
       <c r="L23" s="8"/>
     </row>
     <row r="24" spans="2:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="36" t="s">
+      <c r="B24" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-      <c r="L24" s="38"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="37"/>
     </row>
     <row r="25" spans="2:22" x14ac:dyDescent="0.3">
       <c r="B25" s="21" t="s">
         <v>60</v>
       </c>
       <c r="C25" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="D25" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="E25" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="H25" s="20" t="s">
         <v>61</v>
@@ -1886,13 +1895,13 @@
     </row>
     <row r="26" spans="2:22" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B26" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>45</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>78</v>
@@ -1907,7 +1916,7 @@
     </row>
     <row r="27" spans="2:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B27" s="29" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C27" s="30"/>
       <c r="D27" s="30"/>
@@ -1925,7 +1934,7 @@
         <v>18</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>3</v>
@@ -1934,7 +1943,7 @@
         <v>83</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>14</v>
@@ -1943,7 +1952,7 @@
     </row>
     <row r="29" spans="2:22" ht="33" x14ac:dyDescent="0.3">
       <c r="B29" s="11" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>45</v>
@@ -1968,7 +1977,7 @@
     </row>
     <row r="30" spans="2:22" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B30" s="29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="30"/>
@@ -1986,7 +1995,7 @@
         <v>23</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>5</v>
@@ -2046,17 +2055,17 @@
       <c r="O34" s="30"/>
       <c r="P34" s="31"/>
       <c r="R34" s="29" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="S34" s="30"/>
       <c r="T34" s="31"/>
     </row>
     <row r="35" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B35" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="C35" s="16" t="s">
         <v>27</v>
-      </c>
-      <c r="C35" s="12" t="s">
-        <v>25</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>26</v>
@@ -2094,10 +2103,10 @@
     </row>
     <row r="36" spans="2:24" ht="33" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="s">
-        <v>45</v>
+        <v>137</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>84</v>
+        <v>136</v>
       </c>
       <c r="D36" s="14" t="s">
         <v>45</v>
@@ -2117,7 +2126,7 @@
       <c r="I36" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="J36" s="7"/>
+      <c r="J36" s="14"/>
       <c r="K36" s="7"/>
       <c r="L36" s="8"/>
       <c r="N36" s="11" t="s">
@@ -2170,7 +2179,7 @@
     </row>
     <row r="39" spans="2:24" ht="33" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C39" s="14" t="s">
         <v>45</v>
@@ -2211,9 +2220,9 @@
       </c>
       <c r="O41" s="30"/>
       <c r="P41" s="31"/>
-      <c r="V41" s="32"/>
-      <c r="W41" s="32"/>
-      <c r="X41" s="32"/>
+      <c r="V41" s="38"/>
+      <c r="W41" s="38"/>
+      <c r="X41" s="38"/>
     </row>
     <row r="42" spans="2:24" x14ac:dyDescent="0.3">
       <c r="B42" s="9" t="s">
@@ -2223,19 +2232,19 @@
         <v>37</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="I42" s="1"/>
       <c r="J42" s="2" t="s">
@@ -2267,7 +2276,7 @@
         <v>78</v>
       </c>
       <c r="F43" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G43" s="14" t="s">
         <v>79</v>
@@ -2421,13 +2430,17 @@
     </row>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="V11:X11"/>
-    <mergeCell ref="N18:P18"/>
-    <mergeCell ref="N14:P14"/>
-    <mergeCell ref="B27:L27"/>
-    <mergeCell ref="B21:L21"/>
-    <mergeCell ref="B11:L11"/>
-    <mergeCell ref="B24:L24"/>
+    <mergeCell ref="B44:L44"/>
+    <mergeCell ref="N44:P44"/>
+    <mergeCell ref="V41:X41"/>
+    <mergeCell ref="B47:L47"/>
+    <mergeCell ref="B30:L30"/>
+    <mergeCell ref="B34:L34"/>
+    <mergeCell ref="N34:P34"/>
+    <mergeCell ref="R34:T34"/>
+    <mergeCell ref="B37:L37"/>
+    <mergeCell ref="B41:L41"/>
+    <mergeCell ref="N41:P41"/>
     <mergeCell ref="R2:T2"/>
     <mergeCell ref="R5:T5"/>
     <mergeCell ref="R18:T18"/>
@@ -2439,17 +2452,13 @@
     <mergeCell ref="N8:P8"/>
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="B5:L5"/>
-    <mergeCell ref="B44:L44"/>
-    <mergeCell ref="N44:P44"/>
-    <mergeCell ref="V41:X41"/>
-    <mergeCell ref="B47:L47"/>
-    <mergeCell ref="B30:L30"/>
-    <mergeCell ref="B34:L34"/>
-    <mergeCell ref="N34:P34"/>
-    <mergeCell ref="R34:T34"/>
-    <mergeCell ref="B37:L37"/>
-    <mergeCell ref="B41:L41"/>
-    <mergeCell ref="N41:P41"/>
+    <mergeCell ref="V11:X11"/>
+    <mergeCell ref="N18:P18"/>
+    <mergeCell ref="N14:P14"/>
+    <mergeCell ref="B27:L27"/>
+    <mergeCell ref="B21:L21"/>
+    <mergeCell ref="B11:L11"/>
+    <mergeCell ref="B24:L24"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>